<commit_message>
Updated and added tables to adjust the calculation of PES
</commit_message>
<xml_diff>
--- a/import/raw_data/eurostat/mapping__siec__energy_carrier.xlsx
+++ b/import/raw_data/eurostat/mapping__siec__energy_carrier.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bef\GitHub\micat\import\raw_data\eurostat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A7452F-D064-46EF-BAF1-CFAD8480EDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F226895-ED5F-47E9-9438-40E4505DA1D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="30912" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-1500" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -869,21 +869,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.08984375" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.6328125" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
     <col min="6" max="6" width="61" customWidth="1"/>
-    <col min="10" max="10" width="18.5546875" customWidth="1"/>
+    <col min="10" max="10" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>151</v>
       </c>
@@ -904,7 +904,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -924,7 +924,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -944,7 +944,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -964,7 +964,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -984,7 +984,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>1</v>
       </c>
       <c r="D70">
-        <v>-999</v>
+        <v>7</v>
       </c>
       <c r="E70">
         <v>6000</v>
@@ -2284,7 +2284,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2351,6 +2351,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Type xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">mapping</Type>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010081027A5C4AB68A40A5017F28CDCC410C" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="f1f428d4bdb6f67b400b210b48125618">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ca47701c-f272-4f81-9665-1c7dbebc0776" xmlns:ns3="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8189f6f0f7c839d9d0d3622fd62ec189" ns2:_="" ns3:_="">
     <xsd:import namespace="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
@@ -2603,28 +2624,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A4FEE3C-F8B8-4A41-BBD4-51505283A981}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="89bcd336-abeb-4a08-b6b9-8f1906e00f8a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Type xmlns="ca47701c-f272-4f81-9665-1c7dbebc0776">mapping</Type>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7A11207-9344-4137-9608-88CE20E29773}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{302006AB-AD3B-4051-9A60-1BCC1E8AFA83}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2641,29 +2666,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7A11207-9344-4137-9608-88CE20E29773}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A4FEE3C-F8B8-4A41-BBD4-51505283A981}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="89bcd336-abeb-4a08-b6b9-8f1906e00f8a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>